<commit_message>
Flytt av gamla uppdateringslistor till arkiv
Flytt av gamla uppdateringslistor till arkiv
</commit_message>
<xml_diff>
--- a/Bibsam_tidskriftslistor/scifree_data_oxford.xlsx
+++ b/Bibsam_tidskriftslistor/scifree_data_oxford.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_2BC801F5383D905E5247B3E9B00243C1836B5DFC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4482,7 +4483,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4534,9 +4535,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 7 2" xfId="3"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 7 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -4620,19 +4621,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G476" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:G476"/>
-  <sortState ref="A2:G448">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G476" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:G476" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G448">
     <sortCondition ref="D1:D448"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Imprint"/>
-    <tableColumn id="2" name="ISSN Electronic"/>
-    <tableColumn id="3" name="ISSN Print"/>
-    <tableColumn id="4" name="Journal Name"/>
-    <tableColumn id="5" name="JournalURL"/>
-    <tableColumn id="6" name="Publishing model"/>
-    <tableColumn id="7" name="CC License options"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Imprint"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ISSN Electronic"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ISSN Print"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Journal Name"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="JournalURL"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Publishing model"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CC License options"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4900,10 +4901,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G476"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14590,8 +14593,8 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D340:D1048576 D1:D260">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="B340:B367 B2:B260">
+    <cfRule type="duplicateValues" dxfId="4" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B340:B1048576 B1:B260">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
@@ -14599,11 +14602,11 @@
   <conditionalFormatting sqref="D261:D339">
     <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B340:B367 B2:B260">
-    <cfRule type="duplicateValues" dxfId="1" priority="32"/>
+  <conditionalFormatting sqref="D340:D367 D2:D260">
+    <cfRule type="duplicateValues" dxfId="1" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D340:D367 D2:D260">
-    <cfRule type="duplicateValues" dxfId="0" priority="34"/>
+  <conditionalFormatting sqref="D340:D1048576 D1:D260">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>